<commit_message>
Can create new users using '/userregister' route
</commit_message>
<xml_diff>
--- a/Documents/ER_Inventory/Current-database.xlsx
+++ b/Documents/ER_Inventory/Current-database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Inventory-2k23\Documents\ER_Inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Ongoing-fontend\Documents\ER_Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE709F5B-75B1-4387-8D65-2B9F37445E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B4F43E-7633-4DD3-A129-5D93D0817F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7C6AD97D-0354-4FD0-8E91-EBAC4EC551C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" xr2:uid="{7C6AD97D-0354-4FD0-8E91-EBAC4EC551C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -616,7 +616,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:mm"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +663,29 @@
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -705,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -747,6 +770,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95CA8C8-82BE-40BC-8871-F9C457D45A7D}">
   <dimension ref="A2:T159"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="102" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J2" zoomScale="102" zoomScaleNormal="117" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,7 +1127,7 @@
       <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1133,7 +1163,7 @@
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="20" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="4"/>
@@ -1153,7 +1183,7 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="21" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="2">
@@ -1181,7 +1211,7 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="21" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="2">
@@ -1209,7 +1239,7 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="21" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="2">
@@ -1237,7 +1267,7 @@
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="2">
@@ -1265,7 +1295,7 @@
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="21" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="2">
@@ -1293,7 +1323,7 @@
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="2">
@@ -1321,7 +1351,7 @@
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="21" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="2">

</xml_diff>